<commit_message>
wardope week 10 completed
</commit_message>
<xml_diff>
--- a/controllers/public/reports/sales-report.xlsx
+++ b/controllers/public/reports/sales-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
   <si>
     <t>Order ID</t>
   </si>
@@ -92,6 +92,45 @@
   </si>
   <si>
     <t>12/01/2025, 16:26:09</t>
+  </si>
+  <si>
+    <t>ORD-1736742537979-61cd6af4</t>
+  </si>
+  <si>
+    <t>13/01/2025, 09:58:57</t>
+  </si>
+  <si>
+    <t>ORD-1736742796596-a5238dcc</t>
+  </si>
+  <si>
+    <t>13/01/2025, 10:03:16</t>
+  </si>
+  <si>
+    <t>ORD-1736742919832-eddab4ba</t>
+  </si>
+  <si>
+    <t>13/01/2025, 10:05:19</t>
+  </si>
+  <si>
+    <t>ORD-1736743627086-35daa2b2</t>
+  </si>
+  <si>
+    <t>canceled</t>
+  </si>
+  <si>
+    <t>13/01/2025, 10:17:07</t>
+  </si>
+  <si>
+    <t>ORD-1736743888962-efc6cfe5</t>
+  </si>
+  <si>
+    <t>13/01/2025, 10:21:28</t>
+  </si>
+  <si>
+    <t>ORD-1736744544825-5382ce92</t>
+  </si>
+  <si>
+    <t>13/01/2025, 10:32:24</t>
   </si>
 </sst>
 </file>
@@ -468,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -680,6 +719,180 @@
         <v>26</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>699</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8">
+        <v>699</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>1518</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9">
+        <v>1518</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>759</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10">
+        <v>759</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>709</v>
+      </c>
+      <c r="E11">
+        <v>128</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>581</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>759</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12">
+        <v>759</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>711</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13">
+        <v>711</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
chart updated and categorised
</commit_message>
<xml_diff>
--- a/controllers/public/reports/sales-report.xlsx
+++ b/controllers/public/reports/sales-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="83">
   <si>
     <t>Order ID</t>
   </si>
@@ -178,7 +178,88 @@
     <t>ORD-1736840768506-3f916962</t>
   </si>
   <si>
+    <t>return approved</t>
+  </si>
+  <si>
     <t>14/01/2025, 13:16:08</t>
+  </si>
+  <si>
+    <t>ORD-1736921273602-1d81a9e1</t>
+  </si>
+  <si>
+    <t>15/01/2025, 11:37:53</t>
+  </si>
+  <si>
+    <t>ORD-1736922318507-df33f9bd</t>
+  </si>
+  <si>
+    <t>15/01/2025, 11:55:18</t>
+  </si>
+  <si>
+    <t>ORD-1736922879834-aa9a9186</t>
+  </si>
+  <si>
+    <t>15/01/2025, 12:04:39</t>
+  </si>
+  <si>
+    <t>ORD-1736924311922-71beabcc</t>
+  </si>
+  <si>
+    <t>15/01/2025, 12:28:31</t>
+  </si>
+  <si>
+    <t>ORD-1736924400415-f87fdcf3</t>
+  </si>
+  <si>
+    <t>15/01/2025, 12:30:00</t>
+  </si>
+  <si>
+    <t>ORD-1736950818225-ddb68a48</t>
+  </si>
+  <si>
+    <t>15/01/2025, 19:50:18</t>
+  </si>
+  <si>
+    <t>ORD-1736950882256-eda8eb06</t>
+  </si>
+  <si>
+    <t>15/01/2025, 19:51:22</t>
+  </si>
+  <si>
+    <t>ORD-1737001643934-dcd640af</t>
+  </si>
+  <si>
+    <t>16/01/2025, 09:57:23</t>
+  </si>
+  <si>
+    <t>ORD-1737001988963-2000ff84</t>
+  </si>
+  <si>
+    <t>16/01/2025, 10:03:08</t>
+  </si>
+  <si>
+    <t>ORD-1737005141372-6f847034</t>
+  </si>
+  <si>
+    <t>16/01/2025, 10:55:41</t>
+  </si>
+  <si>
+    <t>ORD-1737005481173-86d4f49c</t>
+  </si>
+  <si>
+    <t>16/01/2025, 11:01:21</t>
+  </si>
+  <si>
+    <t>ORD-1737006109565-f7dead73</t>
+  </si>
+  <si>
+    <t>16/01/2025, 11:11:49</t>
+  </si>
+  <si>
+    <t>ORD-1737006560056-2fbc8a89</t>
+  </si>
+  <si>
+    <t>16/01/2025, 11:19:20</t>
   </si>
 </sst>
 </file>
@@ -555,7 +636,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I32"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -1109,10 +1190,387 @@
         <v>712</v>
       </c>
       <c r="H19" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="I19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>783</v>
+      </c>
+      <c r="E20">
+        <v>196</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20">
+        <v>587</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>712</v>
+      </c>
+      <c r="E21">
+        <v>178</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21">
+        <v>534</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>712</v>
+      </c>
+      <c r="E22">
+        <v>128</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22">
+        <v>712</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>712</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23">
+        <v>712</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>783</v>
+      </c>
+      <c r="E24">
+        <v>141</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24">
+        <v>642</v>
+      </c>
+      <c r="H24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>712</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25">
+        <v>712</v>
+      </c>
+      <c r="H25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>712</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26">
+        <v>712</v>
+      </c>
+      <c r="H26" t="s">
         <v>55</v>
+      </c>
+      <c r="I26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>391</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27">
+        <v>391</v>
+      </c>
+      <c r="H27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>783</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28">
+        <v>783</v>
+      </c>
+      <c r="H28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>712</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29">
+        <v>712</v>
+      </c>
+      <c r="H29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>712</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30">
+        <v>712</v>
+      </c>
+      <c r="H30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>712</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31">
+        <v>712</v>
+      </c>
+      <c r="H31" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>783</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32">
+        <v>783</v>
+      </c>
+      <c r="H32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>